<commit_message>
Removed more apparent duplicates in the data
</commit_message>
<xml_diff>
--- a/data/Pre-Filtered/ratings_data.xlsx
+++ b/data/Pre-Filtered/ratings_data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/coursework/Recommender/data/Pre-Filtered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE47F129-D80D-7A4C-8BED-8F05BF57473F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244BD3C7-4E7F-FC46-B1EF-7119C4BF6591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13540" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContextualRating" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="RatingNew" localSheetId="0">ContextualRating!$A$1:$K$508</definedName>
+    <definedName name="RatingNew" localSheetId="0">ContextualRating!$A$1:$K$506</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D498"/>
+  <dimension ref="A1:D496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A463" workbookViewId="0">
-      <selection activeCell="A491" sqref="A491:A498"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="A220" sqref="A220:XFD220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3430,7 +3430,7 @@
         <v>5</v>
       </c>
       <c r="D213">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -3444,7 +3444,7 @@
         <v>5</v>
       </c>
       <c r="D214">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
@@ -3452,13 +3452,13 @@
         <v>17</v>
       </c>
       <c r="B215">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C215">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D215">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
@@ -3469,10 +3469,10 @@
         <v>278</v>
       </c>
       <c r="C216">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D216">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
@@ -3480,10 +3480,10 @@
         <v>17</v>
       </c>
       <c r="B217">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C217">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D217">
         <v>0</v>
@@ -3494,13 +3494,13 @@
         <v>17</v>
       </c>
       <c r="B218">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C218">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D218">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
@@ -3508,13 +3508,13 @@
         <v>17</v>
       </c>
       <c r="B219">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C219">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D219">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -3528,7 +3528,7 @@
         <v>5</v>
       </c>
       <c r="D220">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
@@ -3536,13 +3536,13 @@
         <v>17</v>
       </c>
       <c r="B221">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C221">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D221">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -3550,13 +3550,13 @@
         <v>17</v>
       </c>
       <c r="B222">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C222">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D222">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -3564,13 +3564,13 @@
         <v>17</v>
       </c>
       <c r="B223">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C223">
         <v>1</v>
       </c>
       <c r="D223">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -3578,7 +3578,7 @@
         <v>17</v>
       </c>
       <c r="B224">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -3592,7 +3592,7 @@
         <v>17</v>
       </c>
       <c r="B225">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -3606,13 +3606,13 @@
         <v>17</v>
       </c>
       <c r="B226">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C226">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D226">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -3620,13 +3620,13 @@
         <v>17</v>
       </c>
       <c r="B227">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C227">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D227">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -3634,13 +3634,13 @@
         <v>17</v>
       </c>
       <c r="B228">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C228">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D228">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
@@ -3648,13 +3648,13 @@
         <v>17</v>
       </c>
       <c r="B229">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C229">
         <v>5</v>
       </c>
       <c r="D229">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -3662,13 +3662,13 @@
         <v>17</v>
       </c>
       <c r="B230">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C230">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D230">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -3676,13 +3676,13 @@
         <v>17</v>
       </c>
       <c r="B231">
-        <v>293</v>
+        <v>676</v>
       </c>
       <c r="C231">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D231">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -3690,10 +3690,10 @@
         <v>17</v>
       </c>
       <c r="B232">
-        <v>296</v>
+        <v>678</v>
       </c>
       <c r="C232">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D232">
         <v>1</v>
@@ -3704,10 +3704,10 @@
         <v>17</v>
       </c>
       <c r="B233">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="C233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D233">
         <v>0</v>
@@ -3718,13 +3718,13 @@
         <v>17</v>
       </c>
       <c r="B234">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="C234">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D234">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -3732,13 +3732,13 @@
         <v>17</v>
       </c>
       <c r="B235">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="C235">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D235">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -3746,13 +3746,13 @@
         <v>17</v>
       </c>
       <c r="B236">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="C236">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D236">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -3760,13 +3760,13 @@
         <v>17</v>
       </c>
       <c r="B237">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="C237">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D237">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
@@ -3774,13 +3774,13 @@
         <v>17</v>
       </c>
       <c r="B238">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="C238">
         <v>1</v>
       </c>
       <c r="D238">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
@@ -3788,13 +3788,13 @@
         <v>17</v>
       </c>
       <c r="B239">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="C239">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D239">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
@@ -3802,13 +3802,13 @@
         <v>17</v>
       </c>
       <c r="B240">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C240">
         <v>1</v>
       </c>
       <c r="D240">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
@@ -3816,13 +3816,13 @@
         <v>17</v>
       </c>
       <c r="B241">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C241">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D241">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -3830,7 +3830,7 @@
         <v>17</v>
       </c>
       <c r="B242">
-        <v>688</v>
+        <v>693</v>
       </c>
       <c r="C242">
         <v>1</v>
@@ -3844,13 +3844,13 @@
         <v>17</v>
       </c>
       <c r="B243">
-        <v>689</v>
+        <v>694</v>
       </c>
       <c r="C243">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D243">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
@@ -3858,7 +3858,7 @@
         <v>17</v>
       </c>
       <c r="B244">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C244">
         <v>1</v>
@@ -3872,13 +3872,13 @@
         <v>17</v>
       </c>
       <c r="B245">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="C245">
         <v>1</v>
       </c>
       <c r="D245">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
@@ -3886,7 +3886,7 @@
         <v>17</v>
       </c>
       <c r="B246">
-        <v>695</v>
+        <v>700</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -3900,13 +3900,13 @@
         <v>17</v>
       </c>
       <c r="B247">
-        <v>697</v>
+        <v>702</v>
       </c>
       <c r="C247">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D247">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -3914,7 +3914,7 @@
         <v>17</v>
       </c>
       <c r="B248">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -3928,13 +3928,13 @@
         <v>17</v>
       </c>
       <c r="B249">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="C249">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D249">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -3942,10 +3942,10 @@
         <v>17</v>
       </c>
       <c r="B250">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C250">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D250">
         <v>2</v>
@@ -3956,7 +3956,7 @@
         <v>17</v>
       </c>
       <c r="B251">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -3970,13 +3970,13 @@
         <v>17</v>
       </c>
       <c r="B252">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C252">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D252">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
@@ -3984,13 +3984,13 @@
         <v>17</v>
       </c>
       <c r="B253">
-        <v>706</v>
+        <v>710</v>
       </c>
       <c r="C253">
         <v>1</v>
       </c>
       <c r="D253">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
@@ -3998,13 +3998,13 @@
         <v>17</v>
       </c>
       <c r="B254">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="C254">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D254">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
@@ -4012,13 +4012,13 @@
         <v>17</v>
       </c>
       <c r="B255">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C255">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D255">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
@@ -4026,13 +4026,13 @@
         <v>17</v>
       </c>
       <c r="B256">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="C256">
         <v>1</v>
       </c>
       <c r="D256">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
@@ -4040,13 +4040,13 @@
         <v>17</v>
       </c>
       <c r="B257">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="C257">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D257">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
@@ -4054,13 +4054,13 @@
         <v>17</v>
       </c>
       <c r="B258">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="C258">
         <v>1</v>
       </c>
       <c r="D258">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
@@ -4068,13 +4068,13 @@
         <v>17</v>
       </c>
       <c r="B259">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C259">
         <v>1</v>
       </c>
       <c r="D259">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
@@ -4082,13 +4082,13 @@
         <v>17</v>
       </c>
       <c r="B260">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C260">
         <v>1</v>
       </c>
       <c r="D260">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
@@ -4096,13 +4096,13 @@
         <v>17</v>
       </c>
       <c r="B261">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="C261">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D261">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
@@ -4110,13 +4110,13 @@
         <v>17</v>
       </c>
       <c r="B262">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="C262">
         <v>1</v>
       </c>
       <c r="D262">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
@@ -4124,13 +4124,13 @@
         <v>17</v>
       </c>
       <c r="B263">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="C263">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D263">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
@@ -4138,13 +4138,13 @@
         <v>17</v>
       </c>
       <c r="B264">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C264">
         <v>1</v>
       </c>
       <c r="D264">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
@@ -4152,10 +4152,10 @@
         <v>17</v>
       </c>
       <c r="B265">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="C265">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D265">
         <v>2</v>
@@ -4166,13 +4166,13 @@
         <v>17</v>
       </c>
       <c r="B266">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="C266">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D266">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
@@ -4180,13 +4180,13 @@
         <v>17</v>
       </c>
       <c r="B267">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C267">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D267">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
@@ -4194,10 +4194,10 @@
         <v>17</v>
       </c>
       <c r="B268">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C268">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D268">
         <v>3</v>
@@ -4208,7 +4208,7 @@
         <v>17</v>
       </c>
       <c r="B269">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C269">
         <v>1</v>
@@ -4222,13 +4222,13 @@
         <v>17</v>
       </c>
       <c r="B270">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="C270">
         <v>1</v>
       </c>
       <c r="D270">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
@@ -4236,7 +4236,7 @@
         <v>17</v>
       </c>
       <c r="B271">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="C271">
         <v>1</v>
@@ -4250,13 +4250,13 @@
         <v>17</v>
       </c>
       <c r="B272">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C272">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D272">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
@@ -4264,13 +4264,13 @@
         <v>17</v>
       </c>
       <c r="B273">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="C273">
         <v>1</v>
       </c>
       <c r="D273">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
@@ -4278,13 +4278,13 @@
         <v>17</v>
       </c>
       <c r="B274">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="C274">
         <v>2</v>
       </c>
       <c r="D274">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
@@ -4292,13 +4292,13 @@
         <v>17</v>
       </c>
       <c r="B275">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C275">
         <v>1</v>
       </c>
       <c r="D275">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
@@ -4306,10 +4306,10 @@
         <v>17</v>
       </c>
       <c r="B276">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="C276">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D276">
         <v>1</v>
@@ -4320,13 +4320,13 @@
         <v>17</v>
       </c>
       <c r="B277">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="C277">
         <v>1</v>
       </c>
       <c r="D277">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
@@ -4334,13 +4334,13 @@
         <v>17</v>
       </c>
       <c r="B278">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C278">
         <v>1</v>
       </c>
       <c r="D278">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
@@ -4348,13 +4348,13 @@
         <v>17</v>
       </c>
       <c r="B279">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="C279">
         <v>1</v>
       </c>
       <c r="D279">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
@@ -4362,13 +4362,13 @@
         <v>17</v>
       </c>
       <c r="B280">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="C280">
         <v>1</v>
       </c>
       <c r="D280">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
@@ -4376,13 +4376,13 @@
         <v>17</v>
       </c>
       <c r="B281">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C281">
         <v>1</v>
       </c>
       <c r="D281">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
@@ -4390,13 +4390,13 @@
         <v>17</v>
       </c>
       <c r="B282">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="C282">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D282">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
@@ -4404,13 +4404,13 @@
         <v>17</v>
       </c>
       <c r="B283">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="C283">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D283">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
@@ -4418,13 +4418,13 @@
         <v>17</v>
       </c>
       <c r="B284">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="C284">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D284">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
@@ -4432,13 +4432,13 @@
         <v>17</v>
       </c>
       <c r="B285">
-        <v>748</v>
+        <v>753</v>
       </c>
       <c r="C285">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D285">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
@@ -4446,13 +4446,13 @@
         <v>17</v>
       </c>
       <c r="B286">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="C286">
         <v>1</v>
       </c>
       <c r="D286">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
@@ -4466,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="D287">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
@@ -4474,13 +4474,13 @@
         <v>17</v>
       </c>
       <c r="B288">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C288">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D288">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
@@ -4488,13 +4488,13 @@
         <v>17</v>
       </c>
       <c r="B289">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="C289">
         <v>1</v>
       </c>
       <c r="D289">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
@@ -4502,13 +4502,13 @@
         <v>17</v>
       </c>
       <c r="B290">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="C290">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D290">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
@@ -4516,13 +4516,13 @@
         <v>17</v>
       </c>
       <c r="B291">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C291">
         <v>1</v>
       </c>
       <c r="D291">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
@@ -4530,13 +4530,13 @@
         <v>17</v>
       </c>
       <c r="B292">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C292">
         <v>1</v>
       </c>
       <c r="D292">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
@@ -4544,13 +4544,13 @@
         <v>17</v>
       </c>
       <c r="B293">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="C293">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D293">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
@@ -4558,13 +4558,13 @@
         <v>17</v>
       </c>
       <c r="B294">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C294">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D294">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
@@ -4572,13 +4572,13 @@
         <v>17</v>
       </c>
       <c r="B295">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C295">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D295">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
@@ -4586,13 +4586,13 @@
         <v>17</v>
       </c>
       <c r="B296">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C296">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D296">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
@@ -4600,41 +4600,41 @@
         <v>17</v>
       </c>
       <c r="B297">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C297">
         <v>1</v>
       </c>
       <c r="D297">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B298">
-        <v>761</v>
+        <v>281</v>
       </c>
       <c r="C298">
         <v>1</v>
       </c>
       <c r="D298">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B299">
-        <v>762</v>
+        <v>296</v>
       </c>
       <c r="C299">
         <v>1</v>
       </c>
       <c r="D299">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
@@ -4642,13 +4642,13 @@
         <v>18</v>
       </c>
       <c r="B300">
-        <v>281</v>
+        <v>684</v>
       </c>
       <c r="C300">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D300">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
@@ -4656,13 +4656,13 @@
         <v>18</v>
       </c>
       <c r="B301">
-        <v>296</v>
+        <v>695</v>
       </c>
       <c r="C301">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D301">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
@@ -4670,10 +4670,10 @@
         <v>18</v>
       </c>
       <c r="B302">
-        <v>684</v>
+        <v>695</v>
       </c>
       <c r="C302">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D302">
         <v>1</v>
@@ -4684,13 +4684,13 @@
         <v>18</v>
       </c>
       <c r="B303">
-        <v>695</v>
+        <v>702</v>
       </c>
       <c r="C303">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D303">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
@@ -4698,13 +4698,13 @@
         <v>18</v>
       </c>
       <c r="B304">
-        <v>695</v>
+        <v>714</v>
       </c>
       <c r="C304">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D304">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
@@ -4712,13 +4712,13 @@
         <v>18</v>
       </c>
       <c r="B305">
-        <v>702</v>
+        <v>722</v>
       </c>
       <c r="C305">
         <v>1</v>
       </c>
       <c r="D305">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
@@ -4726,13 +4726,13 @@
         <v>18</v>
       </c>
       <c r="B306">
-        <v>714</v>
+        <v>725</v>
       </c>
       <c r="C306">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D306">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
@@ -4740,10 +4740,10 @@
         <v>18</v>
       </c>
       <c r="B307">
-        <v>722</v>
+        <v>732</v>
       </c>
       <c r="C307">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D307">
         <v>1</v>
@@ -4754,13 +4754,13 @@
         <v>18</v>
       </c>
       <c r="B308">
-        <v>725</v>
+        <v>737</v>
       </c>
       <c r="C308">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D308">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
@@ -4768,13 +4768,13 @@
         <v>18</v>
       </c>
       <c r="B309">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="C309">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D309">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
@@ -4782,10 +4782,10 @@
         <v>18</v>
       </c>
       <c r="B310">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C310">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -4796,13 +4796,13 @@
         <v>18</v>
       </c>
       <c r="B311">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C311">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D311">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
@@ -4810,10 +4810,10 @@
         <v>18</v>
       </c>
       <c r="B312">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C312">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D312">
         <v>1</v>
@@ -4824,13 +4824,13 @@
         <v>18</v>
       </c>
       <c r="B313">
-        <v>739</v>
+        <v>747</v>
       </c>
       <c r="C313">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D313">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
@@ -4838,41 +4838,41 @@
         <v>18</v>
       </c>
       <c r="B314">
-        <v>739</v>
+        <v>751</v>
       </c>
       <c r="C314">
         <v>0</v>
       </c>
       <c r="D314">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B315">
-        <v>747</v>
+        <v>683</v>
       </c>
       <c r="C315">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D315">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B316">
-        <v>751</v>
+        <v>708</v>
       </c>
       <c r="C316">
         <v>0</v>
       </c>
       <c r="D316">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.2">
@@ -4880,38 +4880,38 @@
         <v>19</v>
       </c>
       <c r="B317">
-        <v>683</v>
+        <v>752</v>
       </c>
       <c r="C317">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D317">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B318">
-        <v>708</v>
+        <v>254</v>
       </c>
       <c r="C318">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D318">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B319">
-        <v>752</v>
+        <v>281</v>
       </c>
       <c r="C319">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D319">
         <v>2</v>
@@ -4922,10 +4922,10 @@
         <v>20</v>
       </c>
       <c r="B320">
-        <v>254</v>
+        <v>678</v>
       </c>
       <c r="C320">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -4936,13 +4936,13 @@
         <v>20</v>
       </c>
       <c r="B321">
-        <v>281</v>
+        <v>710</v>
       </c>
       <c r="C321">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D321">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.2">
@@ -4950,38 +4950,38 @@
         <v>20</v>
       </c>
       <c r="B322">
-        <v>678</v>
+        <v>737</v>
       </c>
       <c r="C322">
         <v>1</v>
       </c>
       <c r="D322">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B323">
-        <v>710</v>
+        <v>251</v>
       </c>
       <c r="C323">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D323">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B324">
-        <v>737</v>
+        <v>252</v>
       </c>
       <c r="C324">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D324">
         <v>2</v>
@@ -4992,10 +4992,10 @@
         <v>21</v>
       </c>
       <c r="B325">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C325">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D325">
         <v>2</v>
@@ -5006,7 +5006,7 @@
         <v>21</v>
       </c>
       <c r="B326">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="C326">
         <v>2</v>
@@ -5020,13 +5020,13 @@
         <v>21</v>
       </c>
       <c r="B327">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="C327">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D327">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
@@ -5034,13 +5034,13 @@
         <v>21</v>
       </c>
       <c r="B328">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C328">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D328">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
@@ -5048,13 +5048,13 @@
         <v>21</v>
       </c>
       <c r="B329">
-        <v>280</v>
+        <v>680</v>
       </c>
       <c r="C329">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D329">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.2">
@@ -5062,13 +5062,13 @@
         <v>21</v>
       </c>
       <c r="B330">
-        <v>282</v>
+        <v>682</v>
       </c>
       <c r="C330">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D330">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.2">
@@ -5076,13 +5076,13 @@
         <v>21</v>
       </c>
       <c r="B331">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="C331">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D331">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.2">
@@ -5090,7 +5090,7 @@
         <v>21</v>
       </c>
       <c r="B332">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="C332">
         <v>4</v>
@@ -5104,13 +5104,13 @@
         <v>21</v>
       </c>
       <c r="B333">
-        <v>684</v>
+        <v>699</v>
       </c>
       <c r="C333">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D333">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.2">
@@ -5118,10 +5118,10 @@
         <v>21</v>
       </c>
       <c r="B334">
-        <v>692</v>
+        <v>699</v>
       </c>
       <c r="C334">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D334">
         <v>0</v>
@@ -5132,13 +5132,13 @@
         <v>21</v>
       </c>
       <c r="B335">
-        <v>699</v>
+        <v>725</v>
       </c>
       <c r="C335">
         <v>2</v>
       </c>
       <c r="D335">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.2">
@@ -5146,13 +5146,13 @@
         <v>21</v>
       </c>
       <c r="B336">
-        <v>699</v>
+        <v>730</v>
       </c>
       <c r="C336">
         <v>5</v>
       </c>
       <c r="D336">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.2">
@@ -5160,13 +5160,13 @@
         <v>21</v>
       </c>
       <c r="B337">
-        <v>725</v>
+        <v>734</v>
       </c>
       <c r="C337">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D337">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.2">
@@ -5174,13 +5174,13 @@
         <v>21</v>
       </c>
       <c r="B338">
-        <v>730</v>
+        <v>750</v>
       </c>
       <c r="C338">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D338">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.2">
@@ -5188,13 +5188,13 @@
         <v>21</v>
       </c>
       <c r="B339">
-        <v>734</v>
+        <v>754</v>
       </c>
       <c r="C339">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D339">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.2">
@@ -5202,41 +5202,41 @@
         <v>21</v>
       </c>
       <c r="B340">
-        <v>750</v>
+        <v>761</v>
       </c>
       <c r="C340">
         <v>2</v>
       </c>
       <c r="D340">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A341">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B341">
-        <v>754</v>
+        <v>259</v>
       </c>
       <c r="C341">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D341">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A342">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B342">
-        <v>761</v>
+        <v>283</v>
       </c>
       <c r="C342">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D342">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.2">
@@ -5244,10 +5244,10 @@
         <v>22</v>
       </c>
       <c r="B343">
-        <v>259</v>
+        <v>705</v>
       </c>
       <c r="C343">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D343">
         <v>2</v>
@@ -5258,69 +5258,69 @@
         <v>22</v>
       </c>
       <c r="B344">
-        <v>283</v>
+        <v>717</v>
       </c>
       <c r="C344">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D344">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A345">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B345">
-        <v>705</v>
+        <v>251</v>
       </c>
       <c r="C345">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D345">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A346">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B346">
-        <v>717</v>
+        <v>291</v>
       </c>
       <c r="C346">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D346">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B347">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="C347">
         <v>5</v>
       </c>
       <c r="D347">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B348">
-        <v>291</v>
+        <v>266</v>
       </c>
       <c r="C348">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D348">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.2">
@@ -5328,13 +5328,13 @@
         <v>24</v>
       </c>
       <c r="B349">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="C349">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D349">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.2">
@@ -5342,13 +5342,13 @@
         <v>24</v>
       </c>
       <c r="B350">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="C350">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D350">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.2">
@@ -5356,13 +5356,13 @@
         <v>24</v>
       </c>
       <c r="B351">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="C351">
         <v>1</v>
       </c>
       <c r="D351">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.2">
@@ -5370,13 +5370,13 @@
         <v>24</v>
       </c>
       <c r="B352">
-        <v>276</v>
+        <v>686</v>
       </c>
       <c r="C352">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D352">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.2">
@@ -5384,13 +5384,13 @@
         <v>24</v>
       </c>
       <c r="B353">
-        <v>290</v>
+        <v>698</v>
       </c>
       <c r="C353">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D353">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.2">
@@ -5398,13 +5398,13 @@
         <v>24</v>
       </c>
       <c r="B354">
-        <v>686</v>
+        <v>731</v>
       </c>
       <c r="C354">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D354">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.2">
@@ -5412,13 +5412,13 @@
         <v>24</v>
       </c>
       <c r="B355">
-        <v>698</v>
+        <v>747</v>
       </c>
       <c r="C355">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D355">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.2">
@@ -5426,24 +5426,24 @@
         <v>24</v>
       </c>
       <c r="B356">
-        <v>731</v>
+        <v>762</v>
       </c>
       <c r="C356">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D356">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B357">
-        <v>747</v>
+        <v>681</v>
       </c>
       <c r="C357">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D357">
         <v>2</v>
@@ -5451,13 +5451,13 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B358">
-        <v>762</v>
+        <v>681</v>
       </c>
       <c r="C358">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D358">
         <v>0</v>
@@ -5468,13 +5468,13 @@
         <v>25</v>
       </c>
       <c r="B359">
-        <v>681</v>
+        <v>712</v>
       </c>
       <c r="C359">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D359">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.2">
@@ -5482,41 +5482,41 @@
         <v>25</v>
       </c>
       <c r="B360">
-        <v>681</v>
+        <v>728</v>
       </c>
       <c r="C360">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D360">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B361">
-        <v>712</v>
+        <v>252</v>
       </c>
       <c r="C361">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D361">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B362">
-        <v>728</v>
+        <v>252</v>
       </c>
       <c r="C362">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D362">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.2">
@@ -5524,7 +5524,7 @@
         <v>26</v>
       </c>
       <c r="B363">
-        <v>252</v>
+        <v>702</v>
       </c>
       <c r="C363">
         <v>1</v>
@@ -5535,30 +5535,30 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B364">
-        <v>252</v>
+        <v>283</v>
       </c>
       <c r="C364">
         <v>1</v>
       </c>
       <c r="D364">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B365">
-        <v>702</v>
+        <v>690</v>
       </c>
       <c r="C365">
         <v>1</v>
       </c>
       <c r="D365">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.2">
@@ -5566,10 +5566,10 @@
         <v>27</v>
       </c>
       <c r="B366">
-        <v>283</v>
+        <v>699</v>
       </c>
       <c r="C366">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D366">
         <v>2</v>
@@ -5580,41 +5580,41 @@
         <v>27</v>
       </c>
       <c r="B367">
-        <v>690</v>
+        <v>745</v>
       </c>
       <c r="C367">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D367">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B368">
-        <v>699</v>
+        <v>687</v>
       </c>
       <c r="C368">
         <v>4</v>
       </c>
       <c r="D368">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A369">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B369">
-        <v>745</v>
+        <v>702</v>
       </c>
       <c r="C369">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D369">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.2">
@@ -5622,13 +5622,13 @@
         <v>28</v>
       </c>
       <c r="B370">
-        <v>687</v>
+        <v>702</v>
       </c>
       <c r="C370">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D370">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.2">
@@ -5636,13 +5636,13 @@
         <v>28</v>
       </c>
       <c r="B371">
-        <v>702</v>
+        <v>725</v>
       </c>
       <c r="C371">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D371">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.2">
@@ -5650,13 +5650,13 @@
         <v>28</v>
       </c>
       <c r="B372">
-        <v>702</v>
+        <v>732</v>
       </c>
       <c r="C372">
         <v>2</v>
       </c>
       <c r="D372">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.2">
@@ -5664,13 +5664,13 @@
         <v>28</v>
       </c>
       <c r="B373">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="C373">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D373">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.2">
@@ -5678,13 +5678,13 @@
         <v>28</v>
       </c>
       <c r="B374">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="C374">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D374">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.2">
@@ -5692,24 +5692,24 @@
         <v>28</v>
       </c>
       <c r="B375">
-        <v>732</v>
+        <v>753</v>
       </c>
       <c r="C375">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D375">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A376">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B376">
-        <v>736</v>
+        <v>254</v>
       </c>
       <c r="C376">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D376">
         <v>1</v>
@@ -5717,13 +5717,13 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A377">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B377">
-        <v>753</v>
+        <v>724</v>
       </c>
       <c r="C377">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D377">
         <v>3</v>
@@ -5734,24 +5734,24 @@
         <v>29</v>
       </c>
       <c r="B378">
-        <v>254</v>
+        <v>739</v>
       </c>
       <c r="C378">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D378">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A379">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B379">
-        <v>724</v>
+        <v>250</v>
       </c>
       <c r="C379">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D379">
         <v>3</v>
@@ -5759,16 +5759,16 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A380">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B380">
-        <v>739</v>
+        <v>252</v>
       </c>
       <c r="C380">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D380">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.2">
@@ -5776,13 +5776,13 @@
         <v>30</v>
       </c>
       <c r="B381">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C381">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D381">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.2">
@@ -5790,13 +5790,13 @@
         <v>30</v>
       </c>
       <c r="B382">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C382">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D382">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.2">
@@ -5804,13 +5804,13 @@
         <v>30</v>
       </c>
       <c r="B383">
-        <v>252</v>
+        <v>675</v>
       </c>
       <c r="C383">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D383">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.2">
@@ -5818,13 +5818,13 @@
         <v>30</v>
       </c>
       <c r="B384">
-        <v>262</v>
+        <v>682</v>
       </c>
       <c r="C384">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D384">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.2">
@@ -5832,13 +5832,13 @@
         <v>30</v>
       </c>
       <c r="B385">
-        <v>675</v>
+        <v>684</v>
       </c>
       <c r="C385">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D385">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
@@ -5846,13 +5846,13 @@
         <v>30</v>
       </c>
       <c r="B386">
-        <v>682</v>
+        <v>705</v>
       </c>
       <c r="C386">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D386">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.2">
@@ -5860,10 +5860,10 @@
         <v>30</v>
       </c>
       <c r="B387">
-        <v>684</v>
+        <v>705</v>
       </c>
       <c r="C387">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D387">
         <v>0</v>
@@ -5874,10 +5874,10 @@
         <v>30</v>
       </c>
       <c r="B388">
-        <v>705</v>
+        <v>724</v>
       </c>
       <c r="C388">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D388">
         <v>2</v>
@@ -5888,7 +5888,7 @@
         <v>30</v>
       </c>
       <c r="B389">
-        <v>705</v>
+        <v>727</v>
       </c>
       <c r="C389">
         <v>4</v>
@@ -5902,13 +5902,13 @@
         <v>30</v>
       </c>
       <c r="B390">
-        <v>724</v>
+        <v>744</v>
       </c>
       <c r="C390">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D390">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.2">
@@ -5916,13 +5916,13 @@
         <v>30</v>
       </c>
       <c r="B391">
-        <v>727</v>
+        <v>744</v>
       </c>
       <c r="C391">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D391">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.2">
@@ -5930,13 +5930,13 @@
         <v>30</v>
       </c>
       <c r="B392">
-        <v>744</v>
+        <v>755</v>
       </c>
       <c r="C392">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D392">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.2">
@@ -5944,10 +5944,10 @@
         <v>30</v>
       </c>
       <c r="B393">
-        <v>744</v>
+        <v>758</v>
       </c>
       <c r="C393">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D393">
         <v>2</v>
@@ -5955,30 +5955,30 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A394">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B394">
-        <v>755</v>
+        <v>251</v>
       </c>
       <c r="C394">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D394">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A395">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B395">
-        <v>758</v>
+        <v>261</v>
       </c>
       <c r="C395">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D395">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.2">
@@ -5986,7 +5986,7 @@
         <v>31</v>
       </c>
       <c r="B396">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="C396">
         <v>3</v>
@@ -6000,7 +6000,7 @@
         <v>31</v>
       </c>
       <c r="B397">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="C397">
         <v>1</v>
@@ -6014,13 +6014,13 @@
         <v>31</v>
       </c>
       <c r="B398">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C398">
         <v>3</v>
       </c>
       <c r="D398">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.2">
@@ -6028,13 +6028,13 @@
         <v>31</v>
       </c>
       <c r="B399">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C399">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D399">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.2">
@@ -6042,13 +6042,13 @@
         <v>31</v>
       </c>
       <c r="B400">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C400">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D400">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.2">
@@ -6056,13 +6056,13 @@
         <v>31</v>
       </c>
       <c r="B401">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="C401">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D401">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.2">
@@ -6070,13 +6070,13 @@
         <v>31</v>
       </c>
       <c r="B402">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C402">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D402">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.2">
@@ -6084,13 +6084,13 @@
         <v>31</v>
       </c>
       <c r="B403">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C403">
         <v>4</v>
       </c>
       <c r="D403">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.2">
@@ -6098,13 +6098,13 @@
         <v>31</v>
       </c>
       <c r="B404">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C404">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D404">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.2">
@@ -6112,13 +6112,13 @@
         <v>31</v>
       </c>
       <c r="B405">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C405">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D405">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.2">
@@ -6126,13 +6126,13 @@
         <v>31</v>
       </c>
       <c r="B406">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C406">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D406">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.2">
@@ -6140,13 +6140,13 @@
         <v>31</v>
       </c>
       <c r="B407">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C407">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D407">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.2">
@@ -6154,13 +6154,13 @@
         <v>31</v>
       </c>
       <c r="B408">
-        <v>291</v>
+        <v>675</v>
       </c>
       <c r="C408">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D408">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.2">
@@ -6168,13 +6168,13 @@
         <v>31</v>
       </c>
       <c r="B409">
-        <v>292</v>
+        <v>676</v>
       </c>
       <c r="C409">
         <v>4</v>
       </c>
       <c r="D409">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.2">
@@ -6182,13 +6182,13 @@
         <v>31</v>
       </c>
       <c r="B410">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="C410">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D410">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.2">
@@ -6196,10 +6196,10 @@
         <v>31</v>
       </c>
       <c r="B411">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="C411">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D411">
         <v>3</v>
@@ -6210,13 +6210,13 @@
         <v>31</v>
       </c>
       <c r="B412">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="C412">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D412">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.2">
@@ -6224,13 +6224,13 @@
         <v>31</v>
       </c>
       <c r="B413">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="C413">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D413">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.2">
@@ -6238,7 +6238,7 @@
         <v>31</v>
       </c>
       <c r="B414">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="C414">
         <v>3</v>
@@ -6252,10 +6252,10 @@
         <v>31</v>
       </c>
       <c r="B415">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="C415">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D415">
         <v>1</v>
@@ -6266,13 +6266,13 @@
         <v>31</v>
       </c>
       <c r="B416">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C416">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D416">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.2">
@@ -6280,10 +6280,10 @@
         <v>31</v>
       </c>
       <c r="B417">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="C417">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D417">
         <v>1</v>
@@ -6294,13 +6294,13 @@
         <v>31</v>
       </c>
       <c r="B418">
-        <v>689</v>
+        <v>694</v>
       </c>
       <c r="C418">
         <v>4</v>
       </c>
       <c r="D418">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.2">
@@ -6308,13 +6308,13 @@
         <v>31</v>
       </c>
       <c r="B419">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="C419">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D419">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.2">
@@ -6322,13 +6322,13 @@
         <v>31</v>
       </c>
       <c r="B420">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="C420">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D420">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.2">
@@ -6336,13 +6336,13 @@
         <v>31</v>
       </c>
       <c r="B421">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="C421">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D421">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.2">
@@ -6350,13 +6350,13 @@
         <v>31</v>
       </c>
       <c r="B422">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="C422">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D422">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.2">
@@ -6364,10 +6364,10 @@
         <v>31</v>
       </c>
       <c r="B423">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="C423">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D423">
         <v>0</v>
@@ -6378,13 +6378,13 @@
         <v>31</v>
       </c>
       <c r="B424">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="C424">
         <v>3</v>
       </c>
       <c r="D424">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.2">
@@ -6392,13 +6392,13 @@
         <v>31</v>
       </c>
       <c r="B425">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="C425">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D425">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.2">
@@ -6406,10 +6406,10 @@
         <v>31</v>
       </c>
       <c r="B426">
-        <v>704</v>
+        <v>717</v>
       </c>
       <c r="C426">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D426">
         <v>3</v>
@@ -6420,13 +6420,13 @@
         <v>31</v>
       </c>
       <c r="B427">
-        <v>707</v>
+        <v>718</v>
       </c>
       <c r="C427">
         <v>5</v>
       </c>
       <c r="D427">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.2">
@@ -6434,13 +6434,13 @@
         <v>31</v>
       </c>
       <c r="B428">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C428">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D428">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.2">
@@ -6448,13 +6448,13 @@
         <v>31</v>
       </c>
       <c r="B429">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C429">
         <v>5</v>
       </c>
       <c r="D429">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.2">
@@ -6462,13 +6462,13 @@
         <v>31</v>
       </c>
       <c r="B430">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C430">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D430">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.2">
@@ -6476,13 +6476,13 @@
         <v>31</v>
       </c>
       <c r="B431">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="C431">
         <v>5</v>
       </c>
       <c r="D431">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.2">
@@ -6490,13 +6490,13 @@
         <v>31</v>
       </c>
       <c r="B432">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C432">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D432">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.2">
@@ -6504,13 +6504,13 @@
         <v>31</v>
       </c>
       <c r="B433">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="C433">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D433">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.2">
@@ -6518,10 +6518,10 @@
         <v>31</v>
       </c>
       <c r="B434">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="C434">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D434">
         <v>1</v>
@@ -6532,13 +6532,13 @@
         <v>31</v>
       </c>
       <c r="B435">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C435">
         <v>4</v>
       </c>
       <c r="D435">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.2">
@@ -6546,13 +6546,13 @@
         <v>31</v>
       </c>
       <c r="B436">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="C436">
         <v>1</v>
       </c>
       <c r="D436">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.2">
@@ -6560,13 +6560,13 @@
         <v>31</v>
       </c>
       <c r="B437">
-        <v>727</v>
+        <v>733</v>
       </c>
       <c r="C437">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D437">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.2">
@@ -6574,13 +6574,13 @@
         <v>31</v>
       </c>
       <c r="B438">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c r="C438">
         <v>1</v>
       </c>
       <c r="D438">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.2">
@@ -6588,13 +6588,13 @@
         <v>31</v>
       </c>
       <c r="B439">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="C439">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D439">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.2">
@@ -6602,13 +6602,13 @@
         <v>31</v>
       </c>
       <c r="B440">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="C440">
         <v>1</v>
       </c>
       <c r="D440">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.2">
@@ -6616,10 +6616,10 @@
         <v>31</v>
       </c>
       <c r="B441">
-        <v>738</v>
+        <v>743</v>
       </c>
       <c r="C441">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D441">
         <v>2</v>
@@ -6630,13 +6630,13 @@
         <v>31</v>
       </c>
       <c r="B442">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="C442">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D442">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.2">
@@ -6644,13 +6644,13 @@
         <v>31</v>
       </c>
       <c r="B443">
-        <v>743</v>
+        <v>751</v>
       </c>
       <c r="C443">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D443">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.2">
@@ -6658,13 +6658,13 @@
         <v>31</v>
       </c>
       <c r="B444">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="C444">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D444">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.2">
@@ -6672,13 +6672,13 @@
         <v>31</v>
       </c>
       <c r="B445">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C445">
         <v>3</v>
       </c>
       <c r="D445">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.2">
@@ -6686,13 +6686,13 @@
         <v>31</v>
       </c>
       <c r="B446">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="C446">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D446">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.2">
@@ -6700,10 +6700,10 @@
         <v>31</v>
       </c>
       <c r="B447">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="C447">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D447">
         <v>0</v>
@@ -6714,13 +6714,13 @@
         <v>31</v>
       </c>
       <c r="B448">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="C448">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D448">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.2">
@@ -6728,13 +6728,13 @@
         <v>31</v>
       </c>
       <c r="B449">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="C449">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D449">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.2">
@@ -6742,13 +6742,13 @@
         <v>31</v>
       </c>
       <c r="B450">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C450">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D450">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.2">
@@ -6756,7 +6756,7 @@
         <v>31</v>
       </c>
       <c r="B451">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C451">
         <v>2</v>
@@ -6770,38 +6770,38 @@
         <v>31</v>
       </c>
       <c r="B452">
-        <v>758</v>
+        <v>762</v>
       </c>
       <c r="C452">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D452">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A453">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B453">
-        <v>759</v>
+        <v>254</v>
       </c>
       <c r="C453">
         <v>2</v>
       </c>
       <c r="D453">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A454">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B454">
-        <v>762</v>
+        <v>284</v>
       </c>
       <c r="C454">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D454">
         <v>3</v>
@@ -6812,13 +6812,13 @@
         <v>32</v>
       </c>
       <c r="B455">
-        <v>254</v>
+        <v>291</v>
       </c>
       <c r="C455">
         <v>2</v>
       </c>
       <c r="D455">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.2">
@@ -6826,13 +6826,13 @@
         <v>32</v>
       </c>
       <c r="B456">
-        <v>284</v>
+        <v>674</v>
       </c>
       <c r="C456">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D456">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.2">
@@ -6840,13 +6840,13 @@
         <v>32</v>
       </c>
       <c r="B457">
-        <v>291</v>
+        <v>683</v>
       </c>
       <c r="C457">
         <v>2</v>
       </c>
       <c r="D457">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.2">
@@ -6854,10 +6854,10 @@
         <v>32</v>
       </c>
       <c r="B458">
-        <v>674</v>
+        <v>704</v>
       </c>
       <c r="C458">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D458">
         <v>2</v>
@@ -6868,13 +6868,13 @@
         <v>32</v>
       </c>
       <c r="B459">
-        <v>683</v>
+        <v>704</v>
       </c>
       <c r="C459">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D459">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.2">
@@ -6882,13 +6882,13 @@
         <v>32</v>
       </c>
       <c r="B460">
-        <v>704</v>
+        <v>730</v>
       </c>
       <c r="C460">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D460">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.2">
@@ -6896,10 +6896,10 @@
         <v>32</v>
       </c>
       <c r="B461">
-        <v>704</v>
+        <v>730</v>
       </c>
       <c r="C461">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D461">
         <v>0</v>
@@ -6910,35 +6910,35 @@
         <v>32</v>
       </c>
       <c r="B462">
-        <v>730</v>
+        <v>758</v>
       </c>
       <c r="C462">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D462">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A463">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B463">
-        <v>730</v>
+        <v>251</v>
       </c>
       <c r="C463">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D463">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A464">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B464">
-        <v>758</v>
+        <v>261</v>
       </c>
       <c r="C464">
         <v>4</v>
@@ -6952,10 +6952,10 @@
         <v>33</v>
       </c>
       <c r="B465">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="C465">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D465">
         <v>1</v>
@@ -6966,13 +6966,13 @@
         <v>33</v>
       </c>
       <c r="B466">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="C466">
         <v>4</v>
       </c>
       <c r="D466">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.2">
@@ -6980,13 +6980,13 @@
         <v>33</v>
       </c>
       <c r="B467">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c r="C467">
         <v>2</v>
       </c>
       <c r="D467">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.2">
@@ -6994,13 +6994,13 @@
         <v>33</v>
       </c>
       <c r="B468">
-        <v>288</v>
+        <v>678</v>
       </c>
       <c r="C468">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D468">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.2">
@@ -7008,13 +7008,13 @@
         <v>33</v>
       </c>
       <c r="B469">
-        <v>297</v>
+        <v>680</v>
       </c>
       <c r="C469">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D469">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.2">
@@ -7022,13 +7022,13 @@
         <v>33</v>
       </c>
       <c r="B470">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="C470">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D470">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.2">
@@ -7036,13 +7036,13 @@
         <v>33</v>
       </c>
       <c r="B471">
-        <v>680</v>
+        <v>685</v>
       </c>
       <c r="C471">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D471">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.2">
@@ -7050,7 +7050,7 @@
         <v>33</v>
       </c>
       <c r="B472">
-        <v>680</v>
+        <v>688</v>
       </c>
       <c r="C472">
         <v>2</v>
@@ -7064,13 +7064,13 @@
         <v>33</v>
       </c>
       <c r="B473">
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="C473">
         <v>2</v>
       </c>
       <c r="D473">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.2">
@@ -7078,13 +7078,13 @@
         <v>33</v>
       </c>
       <c r="B474">
-        <v>688</v>
+        <v>745</v>
       </c>
       <c r="C474">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D474">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.2">
@@ -7092,10 +7092,10 @@
         <v>33</v>
       </c>
       <c r="B475">
-        <v>691</v>
+        <v>749</v>
       </c>
       <c r="C475">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D475">
         <v>0</v>
@@ -7103,30 +7103,30 @@
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A476">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B476">
-        <v>745</v>
+        <v>270</v>
       </c>
       <c r="C476">
         <v>1</v>
       </c>
       <c r="D476">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A477">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B477">
-        <v>749</v>
+        <v>295</v>
       </c>
       <c r="C477">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D477">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.2">
@@ -7134,24 +7134,24 @@
         <v>34</v>
       </c>
       <c r="B478">
-        <v>270</v>
+        <v>680</v>
       </c>
       <c r="C478">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D478">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A479">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B479">
-        <v>295</v>
+        <v>684</v>
       </c>
       <c r="C479">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D479">
         <v>2</v>
@@ -7159,44 +7159,44 @@
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A480">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B480">
-        <v>680</v>
+        <v>692</v>
       </c>
       <c r="C480">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D480">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A481">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B481">
-        <v>684</v>
+        <v>284</v>
       </c>
       <c r="C481">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D481">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A482">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B482">
-        <v>692</v>
+        <v>710</v>
       </c>
       <c r="C482">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D482">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.2">
@@ -7204,13 +7204,13 @@
         <v>36</v>
       </c>
       <c r="B483">
-        <v>284</v>
+        <v>717</v>
       </c>
       <c r="C483">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D483">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.2">
@@ -7218,7 +7218,7 @@
         <v>36</v>
       </c>
       <c r="B484">
-        <v>710</v>
+        <v>721</v>
       </c>
       <c r="C484">
         <v>3</v>
@@ -7229,30 +7229,30 @@
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A485">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B485">
-        <v>717</v>
+        <v>258</v>
       </c>
       <c r="C485">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D485">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A486">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B486">
-        <v>721</v>
+        <v>258</v>
       </c>
       <c r="C486">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D486">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.2">
@@ -7260,38 +7260,38 @@
         <v>37</v>
       </c>
       <c r="B487">
-        <v>258</v>
+        <v>753</v>
       </c>
       <c r="C487">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D487">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A488">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B488">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="C488">
         <v>1</v>
       </c>
       <c r="D488">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A489">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B489">
-        <v>753</v>
+        <v>682</v>
       </c>
       <c r="C489">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D489">
         <v>2</v>
@@ -7299,16 +7299,16 @@
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A490">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B490">
-        <v>285</v>
+        <v>682</v>
       </c>
       <c r="C490">
         <v>1</v>
       </c>
       <c r="D490">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.2">
@@ -7316,13 +7316,13 @@
         <v>39</v>
       </c>
       <c r="B491">
-        <v>682</v>
+        <v>709</v>
       </c>
       <c r="C491">
         <v>1</v>
       </c>
       <c r="D491">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.2">
@@ -7330,7 +7330,7 @@
         <v>39</v>
       </c>
       <c r="B492">
-        <v>682</v>
+        <v>709</v>
       </c>
       <c r="C492">
         <v>1</v>
@@ -7344,13 +7344,13 @@
         <v>39</v>
       </c>
       <c r="B493">
-        <v>709</v>
+        <v>716</v>
       </c>
       <c r="C493">
         <v>1</v>
       </c>
       <c r="D493">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.2">
@@ -7358,13 +7358,13 @@
         <v>39</v>
       </c>
       <c r="B494">
-        <v>709</v>
+        <v>733</v>
       </c>
       <c r="C494">
         <v>1</v>
       </c>
       <c r="D494">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.2">
@@ -7372,13 +7372,13 @@
         <v>39</v>
       </c>
       <c r="B495">
-        <v>716</v>
+        <v>743</v>
       </c>
       <c r="C495">
         <v>1</v>
       </c>
       <c r="D495">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.2">
@@ -7386,45 +7386,17 @@
         <v>39</v>
       </c>
       <c r="B496">
-        <v>733</v>
+        <v>753</v>
       </c>
       <c r="C496">
         <v>1</v>
       </c>
       <c r="D496">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="497" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A497">
-        <v>39</v>
-      </c>
-      <c r="B497">
-        <v>743</v>
-      </c>
-      <c r="C497">
-        <v>1</v>
-      </c>
-      <c r="D497">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="498" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A498">
-        <v>39</v>
-      </c>
-      <c r="B498">
-        <v>753</v>
-      </c>
-      <c r="C498">
-        <v>1</v>
-      </c>
-      <c r="D498">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D498">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D496">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>